<commit_message>
add parsing raw tables (test_importtables.py etc.)
</commit_message>
<xml_diff>
--- a/tests/tbls_test_data/ErrorCodes.xlsx
+++ b/tests/tbls_test_data/ErrorCodes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Box Sync\Projects\Python_ErrorHandling\tests\tbls_test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{001DE2E2-F4EF-4DE3-B52C-14FB5C798703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4241247-927C-4304-B6C2-1F91D57F4F51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1410" yWindow="1410" windowWidth="28800" windowHeight="11332" xr2:uid="{CD3C727C-9923-402D-B728-1749A83ECA6F}"/>
+    <workbookView xWindow="3015" yWindow="2445" windowWidth="27825" windowHeight="16830" xr2:uid="{CD3C727C-9923-402D-B728-1749A83ECA6F}"/>
   </bookViews>
   <sheets>
     <sheet name="Errors_" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="45">
   <si>
     <t>iCode</t>
   </si>
@@ -165,6 +165,12 @@
   </si>
   <si>
     <t>ERROR: tbl1 specified column contains values outside of allowable 0 to 50 range</t>
+  </si>
+  <si>
+    <t>tbl2Procedure</t>
+  </si>
+  <si>
+    <t>ERROR: tbl2 specified column contains values that don't meet required  regex format</t>
   </si>
 </sst>
 </file>
@@ -200,7 +206,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -236,6 +242,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -252,7 +264,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -269,6 +281,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
@@ -587,10 +600,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{616FF38B-CF99-49A7-8EA0-C0A3E18AA1A1}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1105,6 +1118,34 @@
         <v>42</v>
       </c>
     </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A37" s="10">
+        <v>520</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A38" s="10">
+        <v>530</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>